<commit_message>
refer: fetchdatafromexcel using Dataformatter
</commit_message>
<xml_diff>
--- a/exceldata.xlsx
+++ b/exceldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\eclipse-workspace1\AdvanceSeleniumA7\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E481E07-FBB1-4693-9336-1790AA6F442F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ED4AD2-904A-4382-8D58-CFB423892E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>selenium</t>
   </si>
   <si>
     <t>https://www.amazon.com</t>
+  </si>
+  <si>
+    <t>aashi07</t>
+  </si>
+  <si>
+    <t>ashi@123</t>
   </si>
 </sst>
 </file>
@@ -359,37 +365,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D4" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{6AF8D2A1-B8A7-4197-8F50-181ECC25EC8F}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{7C90BA0B-F9BF-4FD0-B031-1E2DD5D37F60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>